<commit_message>
run test by reflection (data from txt, xls, xlsx)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5130ADD6-0093-4EEF-9B37-36C190932116}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>method3</t>
+  </si>
+  <si>
+    <t>method1</t>
+  </si>
+  <si>
+    <t>method2</t>
+  </si>
+  <si>
+    <t>p1;p2</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
   <si>
     <t>Test Class</t>
   </si>
@@ -29,36 +49,12 @@
   </si>
   <si>
     <t>Method Parameters</t>
-  </si>
-  <si>
-    <t>GoogleTest</t>
-  </si>
-  <si>
-    <t>openPageTest</t>
-  </si>
-  <si>
-    <t>yandex</t>
-  </si>
-  <si>
-    <t>YandexTest</t>
-  </si>
-  <si>
-    <t>searchTest</t>
-  </si>
-  <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>yandex;google</t>
-  </si>
-  <si>
-    <t>siteSearchTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,30 +64,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,14 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,11 +365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,214 +377,25 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="257" max="257" width="12.28515625" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" customWidth="1"/>
-    <col min="259" max="259" width="21.85546875" customWidth="1"/>
-    <col min="513" max="513" width="12.28515625" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" customWidth="1"/>
-    <col min="515" max="515" width="21.85546875" customWidth="1"/>
-    <col min="769" max="769" width="12.28515625" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" customWidth="1"/>
-    <col min="771" max="771" width="21.85546875" customWidth="1"/>
-    <col min="1025" max="1025" width="12.28515625" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" customWidth="1"/>
-    <col min="1027" max="1027" width="21.85546875" customWidth="1"/>
-    <col min="1281" max="1281" width="12.28515625" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" customWidth="1"/>
-    <col min="1283" max="1283" width="21.85546875" customWidth="1"/>
-    <col min="1537" max="1537" width="12.28515625" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" customWidth="1"/>
-    <col min="1539" max="1539" width="21.85546875" customWidth="1"/>
-    <col min="1793" max="1793" width="12.28515625" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" customWidth="1"/>
-    <col min="1795" max="1795" width="21.85546875" customWidth="1"/>
-    <col min="2049" max="2049" width="12.28515625" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" customWidth="1"/>
-    <col min="2051" max="2051" width="21.85546875" customWidth="1"/>
-    <col min="2305" max="2305" width="12.28515625" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" customWidth="1"/>
-    <col min="2307" max="2307" width="21.85546875" customWidth="1"/>
-    <col min="2561" max="2561" width="12.28515625" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" customWidth="1"/>
-    <col min="2563" max="2563" width="21.85546875" customWidth="1"/>
-    <col min="2817" max="2817" width="12.28515625" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" customWidth="1"/>
-    <col min="2819" max="2819" width="21.85546875" customWidth="1"/>
-    <col min="3073" max="3073" width="12.28515625" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" customWidth="1"/>
-    <col min="3075" max="3075" width="21.85546875" customWidth="1"/>
-    <col min="3329" max="3329" width="12.28515625" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" customWidth="1"/>
-    <col min="3331" max="3331" width="21.85546875" customWidth="1"/>
-    <col min="3585" max="3585" width="12.28515625" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" customWidth="1"/>
-    <col min="3587" max="3587" width="21.85546875" customWidth="1"/>
-    <col min="3841" max="3841" width="12.28515625" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" customWidth="1"/>
-    <col min="3843" max="3843" width="21.85546875" customWidth="1"/>
-    <col min="4097" max="4097" width="12.28515625" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" customWidth="1"/>
-    <col min="4099" max="4099" width="21.85546875" customWidth="1"/>
-    <col min="4353" max="4353" width="12.28515625" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" customWidth="1"/>
-    <col min="4355" max="4355" width="21.85546875" customWidth="1"/>
-    <col min="4609" max="4609" width="12.28515625" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" customWidth="1"/>
-    <col min="4611" max="4611" width="21.85546875" customWidth="1"/>
-    <col min="4865" max="4865" width="12.28515625" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" customWidth="1"/>
-    <col min="4867" max="4867" width="21.85546875" customWidth="1"/>
-    <col min="5121" max="5121" width="12.28515625" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" customWidth="1"/>
-    <col min="5123" max="5123" width="21.85546875" customWidth="1"/>
-    <col min="5377" max="5377" width="12.28515625" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" customWidth="1"/>
-    <col min="5379" max="5379" width="21.85546875" customWidth="1"/>
-    <col min="5633" max="5633" width="12.28515625" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" customWidth="1"/>
-    <col min="5635" max="5635" width="21.85546875" customWidth="1"/>
-    <col min="5889" max="5889" width="12.28515625" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" customWidth="1"/>
-    <col min="5891" max="5891" width="21.85546875" customWidth="1"/>
-    <col min="6145" max="6145" width="12.28515625" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" customWidth="1"/>
-    <col min="6147" max="6147" width="21.85546875" customWidth="1"/>
-    <col min="6401" max="6401" width="12.28515625" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" customWidth="1"/>
-    <col min="6403" max="6403" width="21.85546875" customWidth="1"/>
-    <col min="6657" max="6657" width="12.28515625" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" customWidth="1"/>
-    <col min="6659" max="6659" width="21.85546875" customWidth="1"/>
-    <col min="6913" max="6913" width="12.28515625" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" customWidth="1"/>
-    <col min="6915" max="6915" width="21.85546875" customWidth="1"/>
-    <col min="7169" max="7169" width="12.28515625" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" customWidth="1"/>
-    <col min="7171" max="7171" width="21.85546875" customWidth="1"/>
-    <col min="7425" max="7425" width="12.28515625" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" customWidth="1"/>
-    <col min="7427" max="7427" width="21.85546875" customWidth="1"/>
-    <col min="7681" max="7681" width="12.28515625" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" customWidth="1"/>
-    <col min="7683" max="7683" width="21.85546875" customWidth="1"/>
-    <col min="7937" max="7937" width="12.28515625" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" customWidth="1"/>
-    <col min="7939" max="7939" width="21.85546875" customWidth="1"/>
-    <col min="8193" max="8193" width="12.28515625" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" customWidth="1"/>
-    <col min="8195" max="8195" width="21.85546875" customWidth="1"/>
-    <col min="8449" max="8449" width="12.28515625" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" customWidth="1"/>
-    <col min="8451" max="8451" width="21.85546875" customWidth="1"/>
-    <col min="8705" max="8705" width="12.28515625" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" customWidth="1"/>
-    <col min="8707" max="8707" width="21.85546875" customWidth="1"/>
-    <col min="8961" max="8961" width="12.28515625" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" customWidth="1"/>
-    <col min="8963" max="8963" width="21.85546875" customWidth="1"/>
-    <col min="9217" max="9217" width="12.28515625" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" customWidth="1"/>
-    <col min="9219" max="9219" width="21.85546875" customWidth="1"/>
-    <col min="9473" max="9473" width="12.28515625" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" customWidth="1"/>
-    <col min="9475" max="9475" width="21.85546875" customWidth="1"/>
-    <col min="9729" max="9729" width="12.28515625" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" customWidth="1"/>
-    <col min="9731" max="9731" width="21.85546875" customWidth="1"/>
-    <col min="9985" max="9985" width="12.28515625" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" customWidth="1"/>
-    <col min="9987" max="9987" width="21.85546875" customWidth="1"/>
-    <col min="10241" max="10241" width="12.28515625" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" customWidth="1"/>
-    <col min="10243" max="10243" width="21.85546875" customWidth="1"/>
-    <col min="10497" max="10497" width="12.28515625" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" customWidth="1"/>
-    <col min="10499" max="10499" width="21.85546875" customWidth="1"/>
-    <col min="10753" max="10753" width="12.28515625" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" customWidth="1"/>
-    <col min="10755" max="10755" width="21.85546875" customWidth="1"/>
-    <col min="11009" max="11009" width="12.28515625" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" customWidth="1"/>
-    <col min="11011" max="11011" width="21.85546875" customWidth="1"/>
-    <col min="11265" max="11265" width="12.28515625" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" customWidth="1"/>
-    <col min="11267" max="11267" width="21.85546875" customWidth="1"/>
-    <col min="11521" max="11521" width="12.28515625" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" customWidth="1"/>
-    <col min="11523" max="11523" width="21.85546875" customWidth="1"/>
-    <col min="11777" max="11777" width="12.28515625" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" customWidth="1"/>
-    <col min="11779" max="11779" width="21.85546875" customWidth="1"/>
-    <col min="12033" max="12033" width="12.28515625" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" customWidth="1"/>
-    <col min="12035" max="12035" width="21.85546875" customWidth="1"/>
-    <col min="12289" max="12289" width="12.28515625" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" customWidth="1"/>
-    <col min="12291" max="12291" width="21.85546875" customWidth="1"/>
-    <col min="12545" max="12545" width="12.28515625" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" customWidth="1"/>
-    <col min="12547" max="12547" width="21.85546875" customWidth="1"/>
-    <col min="12801" max="12801" width="12.28515625" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" customWidth="1"/>
-    <col min="12803" max="12803" width="21.85546875" customWidth="1"/>
-    <col min="13057" max="13057" width="12.28515625" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" customWidth="1"/>
-    <col min="13059" max="13059" width="21.85546875" customWidth="1"/>
-    <col min="13313" max="13313" width="12.28515625" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" customWidth="1"/>
-    <col min="13315" max="13315" width="21.85546875" customWidth="1"/>
-    <col min="13569" max="13569" width="12.28515625" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" customWidth="1"/>
-    <col min="13571" max="13571" width="21.85546875" customWidth="1"/>
-    <col min="13825" max="13825" width="12.28515625" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" customWidth="1"/>
-    <col min="13827" max="13827" width="21.85546875" customWidth="1"/>
-    <col min="14081" max="14081" width="12.28515625" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" customWidth="1"/>
-    <col min="14083" max="14083" width="21.85546875" customWidth="1"/>
-    <col min="14337" max="14337" width="12.28515625" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" customWidth="1"/>
-    <col min="14339" max="14339" width="21.85546875" customWidth="1"/>
-    <col min="14593" max="14593" width="12.28515625" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" customWidth="1"/>
-    <col min="14595" max="14595" width="21.85546875" customWidth="1"/>
-    <col min="14849" max="14849" width="12.28515625" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" customWidth="1"/>
-    <col min="14851" max="14851" width="21.85546875" customWidth="1"/>
-    <col min="15105" max="15105" width="12.28515625" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" customWidth="1"/>
-    <col min="15107" max="15107" width="21.85546875" customWidth="1"/>
-    <col min="15361" max="15361" width="12.28515625" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" customWidth="1"/>
-    <col min="15363" max="15363" width="21.85546875" customWidth="1"/>
-    <col min="15617" max="15617" width="12.28515625" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" customWidth="1"/>
-    <col min="15619" max="15619" width="21.85546875" customWidth="1"/>
-    <col min="15873" max="15873" width="12.28515625" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" customWidth="1"/>
-    <col min="15875" max="15875" width="21.85546875" customWidth="1"/>
-    <col min="16129" max="16129" width="12.28515625" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" customWidth="1"/>
-    <col min="16131" max="16131" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -617,35 +403,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>